<commit_message>
Data&ML: Include AT1 Presentation Slides
</commit_message>
<xml_diff>
--- a/Semester-2/Data-and-Machine-Learning/Assessments/AT1-OptimisingPrice-Presentation/AssessmentTask01_presentation.xlsx
+++ b/Semester-2/Data-and-Machine-Learning/Assessments/AT1-OptimisingPrice-Presentation/AssessmentTask01_presentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\TAFE\Dual-Diploma-2024\Semester-2\Data-and-Machine-Learning\Assessments\AT1-OptimisingPrice-Presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D976122-4454-4474-B7C7-0C9C1E1B30B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D61DBA6-D833-4C4A-A4D2-135C8CD698C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task 1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="57">
   <si>
     <t>Product</t>
   </si>
@@ -246,6 +246,15 @@
   <si>
     <t>TotalCost</t>
   </si>
+  <si>
+    <t>KnownSales</t>
+  </si>
+  <si>
+    <t>LinearInterpolation</t>
+  </si>
+  <si>
+    <t>ForcastLinearInterpolation</t>
+  </si>
 </sst>
 </file>
 
@@ -257,7 +266,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +299,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,7 +393,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -421,6 +437,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -538,6 +555,3714 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="metal"/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7754-4229-A7D6-563DCA544ABE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7754-4229-A7D6-563DCA544ABE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7754-4229-A7D6-563DCA544ABE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$D$2:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>835</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-7754-4229-A7D6-563DCA544ABE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1034529168"/>
+        <c:axId val="1278175440"/>
+        <c:axId val="842463759"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="1034529168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1278175440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1278175440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1034529168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="842463759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1278175440"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="0"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:softEdge rad="38100"/>
+        </a:effectLst>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task 2 &amp; 3'!$C$2:$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-83DB-47D6-BC03-878FC4272E24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="853589087"/>
+        <c:axId val="853586687"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="853589087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="853586687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="853586687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="853589087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task 2 &amp; 3'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KnownSales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-40E6-49AF-83D9-6EA40AE0C1A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task 2 &amp; 3'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LinearInterpolation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-40E6-49AF-83D9-6EA40AE0C1A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Task 2 &amp; 3'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ForcastLinearInterpolation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Task 2 &amp; 3'!$D$2:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>835</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>751</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-40E6-49AF-83D9-6EA40AE0C1A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1514635344"/>
+        <c:axId val="1514636304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1514635344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="320"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1514636304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="20"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1514636304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1514635344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="50"/>
+        <c:minorUnit val="25"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="307">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>465042</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>124385</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>246528</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18DCC359-3908-F7F5-34E2-CBFD1FA80D96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1075765</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>68355</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>168088</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>144555</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7961BDB8-0E03-F43D-3D6A-C388CAFB47F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>117763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>8659</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>3463</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CF8D0B7-017F-A506-5C20-2C4A7B97BB41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,7 +4661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -7269,58 +10994,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2">
         <v>1000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A2, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>959</v>
+      </c>
+      <c r="G2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>110</v>
       </c>
       <c r="B3">
         <v>920</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>920</v>
+      </c>
+      <c r="D3" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A3, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>120</v>
       </c>
       <c r="B4">
         <v>908</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>908</v>
+      </c>
+      <c r="D4" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A4, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>876</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>130</v>
       </c>
       <c r="B5">
         <v>830</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>830</v>
+      </c>
+      <c r="D5" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A5, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>835</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>140</v>
       </c>
@@ -7328,8 +11092,17 @@
         <f>830-(A6-130)*(830-630)/(170-130)</f>
         <v>780</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="8">
+        <f>ROUND(B$5-(A6-A$5)*(B$5-B$9)/(A$9-A$5), 0)</f>
+        <v>780</v>
+      </c>
+      <c r="D6" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A6, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>793</v>
+      </c>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>150</v>
       </c>
@@ -7337,8 +11110,17 @@
         <f>830-(A7-130)*(830-630)/(170-130)</f>
         <v>730</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="8">
+        <f>ROUND(B$5-(A7-A$5)*(B$5-B$9)/(A$9-A$5), 0)</f>
+        <v>730</v>
+      </c>
+      <c r="D7" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A7, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>751</v>
+      </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>160</v>
       </c>
@@ -7346,97 +11128,328 @@
         <f>830-(A8-130)*(830-630)/(170-130)</f>
         <v>680</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="8">
+        <f>ROUND(B$5-(A8-A$5)*(B$5-B$9)/(A$9-A$5), 0)</f>
+        <v>680</v>
+      </c>
+      <c r="D8" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A8, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>710</v>
+      </c>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>170</v>
       </c>
       <c r="B9">
         <v>630</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>630</v>
+      </c>
+      <c r="D9" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A9, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>180</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="8">
+        <f>ROUND($B$9-(A10-$A$9)*($B$9-$B$13)/($A$13-$A$9), 0)</f>
+        <v>601</v>
+      </c>
+      <c r="D10" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A10, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>627</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>190</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="8">
+        <f t="shared" ref="C11:C12" si="0">ROUND($B$9-(A11-$A$9)*($B$9-$B$13)/($A$13-$A$9), 0)</f>
+        <v>573</v>
+      </c>
+      <c r="D11" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A11, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>585</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="8">
+        <f t="shared" si="0"/>
+        <v>544</v>
+      </c>
+      <c r="D12" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A12, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>544</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>210</v>
       </c>
       <c r="B13">
         <v>515</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>515</v>
+      </c>
+      <c r="D13" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A13, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>220</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="8">
+        <f>ROUND($B$13-(A14-$A$13)*($B$13-$B$17)/($A$17-$A$13), 0)</f>
+        <v>469</v>
+      </c>
+      <c r="D14" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A14, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>461</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>230</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="8">
+        <f t="shared" ref="C15:C16" si="1">ROUND($B$13-(A15-$A$13)*($B$13-$B$17)/($A$17-$A$13), 0)</f>
+        <v>423</v>
+      </c>
+      <c r="D15" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A15, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>419</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>240</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="8">
+        <f t="shared" si="1"/>
+        <v>376</v>
+      </c>
+      <c r="D16" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A16, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>378</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>250</v>
       </c>
       <c r="B17">
         <v>330</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>330</v>
+      </c>
+      <c r="D17" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A17, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>260</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="8">
+        <f>ROUND($B$17-(A18-$A$17)*($B$17-$B$20)/($A$20-$A$17), 0)</f>
+        <v>288</v>
+      </c>
+      <c r="D18" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A18, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>294</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>270</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="8">
+        <f>ROUND($B$17-(A19-$A$17)*($B$17-$B$20)/($A$20-$A$17), 0)</f>
+        <v>247</v>
+      </c>
+      <c r="D19" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A19, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>253</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>280</v>
       </c>
       <c r="B20">
         <v>205</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>205</v>
+      </c>
+      <c r="D20" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A20, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>290</v>
       </c>
       <c r="B21">
         <v>190</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>190</v>
+      </c>
+      <c r="D21" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A21, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>300</v>
       </c>
       <c r="B22">
         <v>140</v>
       </c>
+      <c r="C22">
+        <v>140</v>
+      </c>
+      <c r="D22" s="33">
+        <f>ROUND(_xlfn.FORECAST.LINEAR(A22, $E$26:$E$38, $D$26:$D$38), 0)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>100</v>
+      </c>
+      <c r="E26">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>110</v>
+      </c>
+      <c r="E27">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>120</v>
+      </c>
+      <c r="E28">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>130</v>
+      </c>
+      <c r="E29">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>140</v>
+      </c>
+      <c r="E30" s="12">
+        <f>830-(D30-130)*(830-630)/(170-130)</f>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>150</v>
+      </c>
+      <c r="E31" s="12">
+        <f>830-(D31-130)*(830-630)/(170-130)</f>
+        <v>730</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>160</v>
+      </c>
+      <c r="E32" s="12">
+        <f>830-(D32-130)*(830-630)/(170-130)</f>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>170</v>
+      </c>
+      <c r="E33">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>210</v>
+      </c>
+      <c r="E34">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>250</v>
+      </c>
+      <c r="E35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>280</v>
+      </c>
+      <c r="E36">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>290</v>
+      </c>
+      <c r="E37">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>300</v>
+      </c>
+      <c r="E38">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>